<commit_message>
More experiments from Mälardalen matmult
</commit_message>
<xml_diff>
--- a/experiment/xlsx/experiments_Mälardalen.xlsx
+++ b/experiment/xlsx/experiments_Mälardalen.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
   <si>
     <t xml:space="preserve">experiment number</t>
   </si>
@@ -103,13 +103,40 @@
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES1_INPUTSIZE50</t>
   </si>
   <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES1_INPUTSIZE80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES1_INPUTSIZE90</t>
+  </si>
+  <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES1_INPUTSIZE100</t>
   </si>
   <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES1_INPUTSIZE110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES1_INPUTSIZE120</t>
+  </si>
+  <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES1_INPUTSIZE150</t>
   </si>
   <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES1_INPUTSIZE200</t>
+    <t xml:space="preserve">'21'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'32'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES2_WRITEATTACK1_INPUTSIZE100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'211'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'322'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES3_WRITEATTACK1_INPUTSIZE100</t>
   </si>
   <si>
     <t xml:space="preserve">'2111'</t>
@@ -118,19 +145,28 @@
     <t xml:space="preserve">'3222'</t>
   </si>
   <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE100</t>
+  </si>
+  <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE20</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE50</t>
   </si>
   <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE100</t>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE120</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE200</t>
   </si>
 </sst>
 </file>
@@ -273,19 +309,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W81"/>
+  <dimension ref="A1:W84"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="21.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="71.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="71.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.59"/>
@@ -418,19 +454,19 @@
         <v>210000</v>
       </c>
       <c r="R2" s="8" t="n">
-        <v>57031</v>
+        <v>59241</v>
       </c>
       <c r="S2" s="9" t="n">
         <f aca="false">V2/T2</f>
-        <v>210411.881257562</v>
+        <v>202562.414543981</v>
       </c>
       <c r="T2" s="8" t="n">
         <f aca="false">R2/10</f>
-        <v>5703.1</v>
+        <v>5924.1</v>
       </c>
       <c r="U2" s="3" t="n">
         <f aca="false">R2/(V2/Q2)</f>
-        <v>9.980425</v>
+        <v>10.367175</v>
       </c>
       <c r="V2" s="1" t="n">
         <v>1200000000</v>
@@ -489,26 +525,26 @@
         <v>15000</v>
       </c>
       <c r="R3" s="8" t="n">
-        <v>808252</v>
+        <v>807727</v>
       </c>
       <c r="S3" s="9" t="n">
         <f aca="false">V3/T3</f>
-        <v>14846.8546938331</v>
+        <v>14856.5047348919</v>
       </c>
       <c r="T3" s="8" t="n">
         <f aca="false">R3/10</f>
-        <v>80825.2</v>
+        <v>80772.7</v>
       </c>
       <c r="U3" s="3" t="n">
         <f aca="false">R3/(V3/Q3)</f>
-        <v>10.10315</v>
+        <v>10.0965875</v>
       </c>
       <c r="V3" s="1" t="n">
         <v>1200000000</v>
       </c>
       <c r="W3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <f aca="false">A3+1</f>
         <v>3</v>
@@ -554,31 +590,32 @@
         <v>0</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="Q4" s="8" t="n">
-        <v>1700</v>
+        <v>3700</v>
       </c>
       <c r="R4" s="8" t="n">
-        <v>7212237</v>
+        <v>3264250</v>
       </c>
       <c r="S4" s="9" t="n">
         <f aca="false">V4/T4</f>
-        <v>1663.83883391519</v>
+        <v>3676.18901738531</v>
       </c>
       <c r="T4" s="8" t="n">
         <f aca="false">R4/10</f>
-        <v>721223.7</v>
+        <v>326425</v>
       </c>
       <c r="U4" s="3" t="n">
         <f aca="false">R4/(V4/Q4)</f>
-        <v>10.21733575</v>
+        <v>10.0647708333333</v>
       </c>
       <c r="V4" s="1" t="n">
         <v>1200000000</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W4" s="0"/>
+    </row>
+    <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <f aca="false">A4+1</f>
         <v>4</v>
@@ -624,29 +661,30 @@
         <v>0</v>
       </c>
       <c r="P5" s="1" t="n">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="Q5" s="8" t="n">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="R5" s="8" t="n">
-        <v>26879304</v>
+        <v>4815093</v>
       </c>
       <c r="S5" s="9" t="n">
         <f aca="false">V5/T5</f>
-        <v>446.440131039107</v>
+        <v>2492.16370275714</v>
       </c>
       <c r="T5" s="8" t="n">
         <f aca="false">R5/10</f>
-        <v>2687930.4</v>
+        <v>481509.3</v>
       </c>
       <c r="U5" s="3" t="n">
         <f aca="false">R5/(V5/Q5)</f>
-        <v>11.19971</v>
+        <v>10.03144375</v>
       </c>
       <c r="V5" s="1" t="n">
         <v>1200000000</v>
       </c>
+      <c r="W5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -694,25 +732,25 @@
         <v>0</v>
       </c>
       <c r="P6" s="1" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q6" s="8" t="n">
-        <v>200</v>
+        <v>1700</v>
       </c>
       <c r="R6" s="8" t="n">
-        <v>63790092</v>
+        <v>7216763</v>
       </c>
       <c r="S6" s="9" t="n">
         <f aca="false">V6/T6</f>
-        <v>188.116988450181</v>
+        <v>1662.79535575714</v>
       </c>
       <c r="T6" s="8" t="n">
         <f aca="false">R6/10</f>
-        <v>6379009.2</v>
+        <v>721676.3</v>
       </c>
       <c r="U6" s="3" t="n">
         <f aca="false">R6/(V6/Q6)</f>
-        <v>10.631682</v>
+        <v>10.2237475833333</v>
       </c>
       <c r="V6" s="1" t="n">
         <v>1200000000</v>
@@ -723,11 +761,11 @@
         <f aca="false">A6+1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
+      <c r="B7" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D7" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -749,20 +787,14 @@
         <v>1048576</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
       <c r="N7" s="0" t="n">
         <v>0</v>
       </c>
@@ -770,11 +802,28 @@
         <v>0</v>
       </c>
       <c r="P7" s="1" t="n">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="Q7" s="8" t="n">
-        <f aca="false">Q$2</f>
-        <v>210000</v>
+        <v>1300</v>
+      </c>
+      <c r="R7" s="8" t="n">
+        <v>9600786</v>
+      </c>
+      <c r="S7" s="9" t="n">
+        <f aca="false">V7/T7</f>
+        <v>1249.89766462871</v>
+      </c>
+      <c r="T7" s="8" t="n">
+        <f aca="false">R7/10</f>
+        <v>960078.6</v>
+      </c>
+      <c r="U7" s="3" t="n">
+        <f aca="false">R7/(V7/Q7)</f>
+        <v>10.4008515</v>
+      </c>
+      <c r="V7" s="1" t="n">
+        <v>1200000000</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,11 +831,11 @@
         <f aca="false">A7+1</f>
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
+      <c r="B8" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D8" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -808,20 +857,14 @@
         <v>1048576</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
       <c r="N8" s="0" t="n">
         <v>0</v>
       </c>
@@ -829,11 +872,28 @@
         <v>0</v>
       </c>
       <c r="P8" s="1" t="n">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="Q8" s="8" t="n">
-        <f aca="false">Q$3</f>
-        <v>15000</v>
+        <v>1000</v>
+      </c>
+      <c r="R8" s="8" t="n">
+        <v>13128562</v>
+      </c>
+      <c r="S8" s="9" t="n">
+        <f aca="false">V8/T8</f>
+        <v>914.037653171764</v>
+      </c>
+      <c r="T8" s="8" t="n">
+        <f aca="false">R8/10</f>
+        <v>1312856.2</v>
+      </c>
+      <c r="U8" s="3" t="n">
+        <f aca="false">R8/(V8/Q8)</f>
+        <v>10.9404683333333</v>
+      </c>
+      <c r="V8" s="1" t="n">
+        <v>1200000000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -841,11 +901,11 @@
         <f aca="false">A8+1</f>
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>30</v>
+      <c r="B9" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D9" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -867,20 +927,14 @@
         <v>1048576</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
       <c r="N9" s="0" t="n">
         <v>0</v>
       </c>
@@ -888,11 +942,28 @@
         <v>0</v>
       </c>
       <c r="P9" s="1" t="n">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="Q9" s="8" t="n">
-        <f aca="false">Q$4</f>
-        <v>1700</v>
+        <v>450</v>
+      </c>
+      <c r="R9" s="8" t="n">
+        <v>26884757</v>
+      </c>
+      <c r="S9" s="9" t="n">
+        <f aca="false">V9/T9</f>
+        <v>446.349580172884</v>
+      </c>
+      <c r="T9" s="8" t="n">
+        <f aca="false">R9/10</f>
+        <v>2688475.7</v>
+      </c>
+      <c r="U9" s="3" t="n">
+        <f aca="false">R9/(V9/Q9)</f>
+        <v>10.081783875</v>
+      </c>
+      <c r="V9" s="1" t="n">
+        <v>1200000000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,10 +972,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D10" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -934,12 +1005,8 @@
       <c r="K10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
       <c r="N10" s="0" t="n">
         <v>0</v>
       </c>
@@ -947,11 +1014,11 @@
         <v>0</v>
       </c>
       <c r="P10" s="1" t="n">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="Q10" s="8" t="n">
-        <f aca="false">Q$5</f>
-        <v>500</v>
+        <f aca="false">Q$6</f>
+        <v>1700</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -960,10 +1027,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D11" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -985,7 +1052,7 @@
         <v>1048576</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>25</v>
@@ -996,9 +1063,7 @@
       <c r="L11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="M11" s="1"/>
       <c r="N11" s="0" t="n">
         <v>0</v>
       </c>
@@ -1006,267 +1071,591 @@
         <v>0</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="Q11" s="8" t="n">
         <f aca="false">Q$6</f>
-        <v>200</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="A12" s="0" t="n">
+        <f aca="false">A11+1</f>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F12" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q12" s="8" t="n">
+        <f aca="false">Q$6</f>
+        <v>1700</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+      <c r="A13" s="0" t="n">
+        <f aca="false">A12+1</f>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="8" t="n">
+        <f aca="false">Q$2</f>
+        <v>210000</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="A14" s="0" t="n">
+        <f aca="false">A13+1</f>
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="8" t="n">
+        <f aca="false">Q$3</f>
+        <v>15000</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="A15" s="0" t="n">
+        <f aca="false">A14+1</f>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q15" s="8" t="n">
+        <f aca="false">Q$4</f>
+        <v>3700</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="A16" s="0" t="n">
+        <f aca="false">A15+1</f>
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q16" s="8" t="n">
+        <f aca="false">Q$5</f>
+        <v>2500</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="A17" s="0" t="n">
+        <f aca="false">A16+1</f>
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G17" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q17" s="8" t="n">
+        <f aca="false">Q$6</f>
+        <v>1700</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="A18" s="0" t="n">
+        <f aca="false">A17+1</f>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G18" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q18" s="8" t="n">
+        <f aca="false">Q$7</f>
+        <v>1300</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+      <c r="A19" s="0" t="n">
+        <f aca="false">A18+1</f>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P19" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q19" s="8" t="n">
+        <f aca="false">Q$8</f>
+        <v>1000</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="A20" s="0" t="n">
+        <f aca="false">A19+1</f>
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F20" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G20" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="Q20" s="8" t="n">
+        <f aca="false">Q$9</f>
+        <v>450</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
+      <c r="S21" s="0"/>
+      <c r="U21" s="0"/>
+      <c r="V21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="S22" s="0"/>
+      <c r="U22" s="0"/>
+      <c r="V22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
+      <c r="S23" s="0"/>
+      <c r="U23" s="0"/>
+      <c r="V23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
+      <c r="S24" s="0"/>
+      <c r="U24" s="0"/>
+      <c r="V24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
+      <c r="S25" s="0"/>
+      <c r="U25" s="0"/>
+      <c r="V25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
+      <c r="S26" s="0"/>
+      <c r="U26" s="0"/>
+      <c r="V26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
+      <c r="S27" s="0"/>
+      <c r="U27" s="0"/>
+      <c r="V27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
+      <c r="S28" s="0"/>
+      <c r="U28" s="0"/>
+      <c r="V28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
@@ -2063,6 +2452,51 @@
       <c r="O81" s="1"/>
       <c r="P81" s="1"/>
     </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="J82" s="1"/>
+      <c r="K82" s="1"/>
+      <c r="L82" s="1"/>
+      <c r="M82" s="1"/>
+      <c r="O82" s="1"/>
+      <c r="P82" s="1"/>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="J83" s="1"/>
+      <c r="K83" s="1"/>
+      <c r="L83" s="1"/>
+      <c r="M83" s="1"/>
+      <c r="O83" s="1"/>
+      <c r="P83" s="1"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="J84" s="1"/>
+      <c r="K84" s="1"/>
+      <c r="L84" s="1"/>
+      <c r="M84" s="1"/>
+      <c r="O84" s="1"/>
+      <c r="P84" s="1"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Corrected errors in xlsx configuration
</commit_message>
<xml_diff>
--- a/experiment/xlsx/experiments_Mälardalen.xlsx
+++ b/experiment/xlsx/experiments_Mälardalen.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="69">
   <si>
     <t xml:space="preserve">experiment number</t>
   </si>
@@ -91,15 +91,39 @@
     <t xml:space="preserve">'2'</t>
   </si>
   <si>
+    <t xml:space="preserve">'1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'4679'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE6000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT_CORES1_INPUTSIZE8000</t>
+  </si>
+  <si>
     <t xml:space="preserve">'3'</t>
   </si>
   <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES1_INPUTSIZE20</t>
   </si>
   <si>
-    <t xml:space="preserve">'4679'</t>
-  </si>
-  <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES1_INPUTSIZE50</t>
   </si>
   <si>
@@ -148,6 +172,24 @@
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE100</t>
   </si>
   <si>
+    <t xml:space="preserve">'12'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT100_CORES2_WRITEATTACK1_INPUTSIZE2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'122'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT100_CORES3_WRITEATTACK1_INPUTSIZE2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'1222'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT100_CORES4_WRITEATTACK1_INPUTSIZE2000</t>
+  </si>
+  <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE20</t>
   </si>
   <si>
@@ -167,6 +209,24 @@
   </si>
   <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT100_CORES4_WRITEATTACK1_INPUTSIZE100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT100_CORES4_WRITEATTACK1_INPUTSIZE500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT100_CORES4_WRITEATTACK1_INPUTSIZE1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT100_CORES4_WRITEATTACK1_INPUTSIZE4000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT100_CORES4_WRITEATTACK1_INPUTSIZE6000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_BSORT100_CORES4_WRITEATTACK1_INPUTSIZE8000</t>
   </si>
 </sst>
 </file>
@@ -312,16 +372,16 @@
   <dimension ref="A1:W84"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="21.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="71.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="74.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="10" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.59"/>
@@ -438,35 +498,35 @@
       <c r="J2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
       <c r="N2" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O2" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P2" s="1" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="8" t="n">
-        <v>210000</v>
+        <v>10000</v>
       </c>
       <c r="R2" s="8" t="n">
-        <v>59241</v>
+        <v>58929</v>
       </c>
       <c r="S2" s="9" t="n">
         <f aca="false">V2/T2</f>
-        <v>202562.414543981</v>
+        <v>203634.882655399</v>
       </c>
       <c r="T2" s="8" t="n">
         <f aca="false">R2/10</f>
-        <v>5924.1</v>
+        <v>5892.9</v>
       </c>
       <c r="U2" s="3" t="n">
         <f aca="false">R2/(V2/Q2)</f>
-        <v>10.367175</v>
+        <v>0.491075</v>
       </c>
       <c r="V2" s="1" t="n">
         <v>1200000000</v>
@@ -509,35 +569,35 @@
       <c r="J3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
       <c r="N3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O3" s="1" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="P3" s="1" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="Q3" s="8" t="n">
-        <v>15000</v>
+        <v>9000</v>
       </c>
       <c r="R3" s="8" t="n">
-        <v>807727</v>
+        <v>1346436</v>
       </c>
       <c r="S3" s="9" t="n">
         <f aca="false">V3/T3</f>
-        <v>14856.5047348919</v>
+        <v>8912.41767154176</v>
       </c>
       <c r="T3" s="8" t="n">
         <f aca="false">R3/10</f>
-        <v>80772.7</v>
+        <v>134643.6</v>
       </c>
       <c r="U3" s="3" t="n">
         <f aca="false">R3/(V3/Q3)</f>
-        <v>10.0965875</v>
+        <v>10.09827</v>
       </c>
       <c r="V3" s="1" t="n">
         <v>1200000000</v>
@@ -580,35 +640,35 @@
       <c r="J4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
       <c r="N4" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O4" s="1" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="P4" s="1" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="8" t="n">
-        <v>3700</v>
+        <v>2250</v>
       </c>
       <c r="R4" s="8" t="n">
-        <v>3264250</v>
+        <v>5355925</v>
       </c>
       <c r="S4" s="9" t="n">
         <f aca="false">V4/T4</f>
-        <v>3676.18901738531</v>
+        <v>2240.50934245719</v>
       </c>
       <c r="T4" s="8" t="n">
         <f aca="false">R4/10</f>
-        <v>326425</v>
+        <v>535592.5</v>
       </c>
       <c r="U4" s="3" t="n">
         <f aca="false">R4/(V4/Q4)</f>
-        <v>10.0647708333333</v>
+        <v>10.042359375</v>
       </c>
       <c r="V4" s="1" t="n">
         <v>1200000000</v>
@@ -651,35 +711,35 @@
       <c r="J5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
       <c r="N5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O5" s="1" t="n">
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="P5" s="1" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="8" t="n">
-        <v>2500</v>
+        <v>600</v>
       </c>
       <c r="R5" s="8" t="n">
-        <v>4815093</v>
+        <v>21262688</v>
       </c>
       <c r="S5" s="9" t="n">
         <f aca="false">V5/T5</f>
-        <v>2492.16370275714</v>
+        <v>564.368907637642</v>
       </c>
       <c r="T5" s="8" t="n">
         <f aca="false">R5/10</f>
-        <v>481509.3</v>
+        <v>2126268.8</v>
       </c>
       <c r="U5" s="3" t="n">
         <f aca="false">R5/(V5/Q5)</f>
-        <v>10.03144375</v>
+        <v>10.631344</v>
       </c>
       <c r="V5" s="1" t="n">
         <v>1200000000</v>
@@ -722,35 +782,32 @@
       <c r="J6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
       <c r="N6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O6" s="1" t="n">
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="P6" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="8" t="n">
-        <v>1700</v>
+        <v>150</v>
       </c>
       <c r="R6" s="8" t="n">
-        <v>7216763</v>
+        <v>84496533</v>
       </c>
       <c r="S6" s="9" t="n">
         <f aca="false">V6/T6</f>
-        <v>1662.79535575714</v>
+        <v>142.017661245344</v>
       </c>
       <c r="T6" s="8" t="n">
         <f aca="false">R6/10</f>
-        <v>721676.3</v>
+        <v>8449653.3</v>
       </c>
       <c r="U6" s="3" t="n">
         <f aca="false">R6/(V6/Q6)</f>
-        <v>10.2237475833333</v>
+        <v>10.562066625</v>
       </c>
       <c r="V6" s="1" t="n">
         <v>1200000000</v>
@@ -792,35 +849,32 @@
       <c r="J7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
       <c r="N7" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O7" s="1" t="n">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="P7" s="1" t="n">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="Q7" s="8" t="n">
-        <v>1300</v>
+        <v>65</v>
       </c>
       <c r="R7" s="8" t="n">
-        <v>9600786</v>
+        <v>189723795</v>
       </c>
       <c r="S7" s="9" t="n">
         <f aca="false">V7/T7</f>
-        <v>1249.89766462871</v>
+        <v>63.2498416975056</v>
       </c>
       <c r="T7" s="8" t="n">
         <f aca="false">R7/10</f>
-        <v>960078.6</v>
+        <v>18972379.5</v>
       </c>
       <c r="U7" s="3" t="n">
         <f aca="false">R7/(V7/Q7)</f>
-        <v>10.4008515</v>
+        <v>10.2767055625</v>
       </c>
       <c r="V7" s="1" t="n">
         <v>1200000000</v>
@@ -862,35 +916,32 @@
       <c r="J8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
       <c r="N8" s="0" t="n">
         <v>0</v>
       </c>
       <c r="O8" s="1" t="n">
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="P8" s="1" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="Q8" s="8" t="n">
-        <v>1000</v>
+        <v>40</v>
       </c>
       <c r="R8" s="8" t="n">
-        <v>13128562</v>
+        <v>337052981</v>
       </c>
       <c r="S8" s="9" t="n">
         <f aca="false">V8/T8</f>
-        <v>914.037653171764</v>
+        <v>35.6027113731417</v>
       </c>
       <c r="T8" s="8" t="n">
         <f aca="false">R8/10</f>
-        <v>1312856.2</v>
+        <v>33705298.1</v>
       </c>
       <c r="U8" s="3" t="n">
         <f aca="false">R8/(V8/Q8)</f>
-        <v>10.9404683333333</v>
+        <v>11.2350993666667</v>
       </c>
       <c r="V8" s="1" t="n">
         <v>1200000000</v>
@@ -905,7 +956,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D9" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -927,7 +978,7 @@
         <v>1048576</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>25</v>
@@ -942,25 +993,25 @@
         <v>0</v>
       </c>
       <c r="P9" s="1" t="n">
-        <v>150</v>
+        <v>20</v>
       </c>
       <c r="Q9" s="8" t="n">
-        <v>450</v>
+        <v>210000</v>
       </c>
       <c r="R9" s="8" t="n">
-        <v>26884757</v>
+        <v>59241</v>
       </c>
       <c r="S9" s="9" t="n">
         <f aca="false">V9/T9</f>
-        <v>446.349580172884</v>
+        <v>202562.414543981</v>
       </c>
       <c r="T9" s="8" t="n">
         <f aca="false">R9/10</f>
-        <v>2688475.7</v>
+        <v>5924.1</v>
       </c>
       <c r="U9" s="3" t="n">
         <f aca="false">R9/(V9/Q9)</f>
-        <v>10.081783875</v>
+        <v>10.367175</v>
       </c>
       <c r="V9" s="1" t="n">
         <v>1200000000</v>
@@ -971,54 +1022,69 @@
         <f aca="false">A9+1</f>
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
+      <c r="B10" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E10" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F10" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G10" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="0" t="n">
-        <v>1048576</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="J10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O10" s="0" t="n">
+      <c r="O10" s="1" t="n">
         <v>0</v>
       </c>
       <c r="P10" s="1" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="Q10" s="8" t="n">
-        <f aca="false">Q$6</f>
-        <v>1700</v>
+        <v>15000</v>
+      </c>
+      <c r="R10" s="8" t="n">
+        <v>807727</v>
+      </c>
+      <c r="S10" s="9" t="n">
+        <f aca="false">V10/T10</f>
+        <v>14856.5047348919</v>
+      </c>
+      <c r="T10" s="8" t="n">
+        <f aca="false">R10/10</f>
+        <v>80772.7</v>
+      </c>
+      <c r="U10" s="3" t="n">
+        <f aca="false">R10/(V10/Q10)</f>
+        <v>10.0965875</v>
+      </c>
+      <c r="V10" s="1" t="n">
+        <v>1200000000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1026,11 +1092,11 @@
         <f aca="false">A10+1</f>
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>36</v>
+      <c r="B11" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1052,30 +1118,43 @@
         <v>1048576</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="O11" s="1" t="n">
         <v>0</v>
       </c>
       <c r="P11" s="1" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="Q11" s="8" t="n">
-        <f aca="false">Q$6</f>
-        <v>1700</v>
+        <v>3700</v>
+      </c>
+      <c r="R11" s="8" t="n">
+        <v>3264250</v>
+      </c>
+      <c r="S11" s="9" t="n">
+        <f aca="false">V11/T11</f>
+        <v>3676.18901738531</v>
+      </c>
+      <c r="T11" s="8" t="n">
+        <f aca="false">R11/10</f>
+        <v>326425</v>
+      </c>
+      <c r="U11" s="3" t="n">
+        <f aca="false">R11/(V11/Q11)</f>
+        <v>10.0647708333333</v>
+      </c>
+      <c r="V11" s="1" t="n">
+        <v>1200000000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,11 +1162,11 @@
         <f aca="false">A11+1</f>
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>39</v>
+      <c r="B12" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D12" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1109,32 +1188,43 @@
         <v>1048576</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
       <c r="N12" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="O12" s="1" t="n">
         <v>0</v>
       </c>
       <c r="P12" s="1" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Q12" s="8" t="n">
-        <f aca="false">Q$6</f>
-        <v>1700</v>
+        <v>2500</v>
+      </c>
+      <c r="R12" s="8" t="n">
+        <v>4815093</v>
+      </c>
+      <c r="S12" s="9" t="n">
+        <f aca="false">V12/T12</f>
+        <v>2492.16370275714</v>
+      </c>
+      <c r="T12" s="8" t="n">
+        <f aca="false">R12/10</f>
+        <v>481509.3</v>
+      </c>
+      <c r="U12" s="3" t="n">
+        <f aca="false">R12/(V12/Q12)</f>
+        <v>10.03144375</v>
+      </c>
+      <c r="V12" s="1" t="n">
+        <v>1200000000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,11 +1232,11 @@
         <f aca="false">A12+1</f>
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>39</v>
+      <c r="B13" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D13" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1168,20 +1258,14 @@
         <v>1048576</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
       <c r="N13" s="0" t="n">
         <v>0</v>
       </c>
@@ -1189,11 +1273,28 @@
         <v>0</v>
       </c>
       <c r="P13" s="1" t="n">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="Q13" s="8" t="n">
-        <f aca="false">Q$2</f>
-        <v>210000</v>
+        <v>1700</v>
+      </c>
+      <c r="R13" s="8" t="n">
+        <v>7216763</v>
+      </c>
+      <c r="S13" s="9" t="n">
+        <f aca="false">V13/T13</f>
+        <v>1662.79535575714</v>
+      </c>
+      <c r="T13" s="8" t="n">
+        <f aca="false">R13/10</f>
+        <v>721676.3</v>
+      </c>
+      <c r="U13" s="3" t="n">
+        <f aca="false">R13/(V13/Q13)</f>
+        <v>10.2237475833333</v>
+      </c>
+      <c r="V13" s="1" t="n">
+        <v>1200000000</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1201,11 +1302,11 @@
         <f aca="false">A13+1</f>
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
+      <c r="B14" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D14" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1227,20 +1328,14 @@
         <v>1048576</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
       <c r="N14" s="0" t="n">
         <v>0</v>
       </c>
@@ -1248,11 +1343,28 @@
         <v>0</v>
       </c>
       <c r="P14" s="1" t="n">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="Q14" s="8" t="n">
-        <f aca="false">Q$3</f>
-        <v>15000</v>
+        <v>1300</v>
+      </c>
+      <c r="R14" s="8" t="n">
+        <v>9600786</v>
+      </c>
+      <c r="S14" s="9" t="n">
+        <f aca="false">V14/T14</f>
+        <v>1249.89766462871</v>
+      </c>
+      <c r="T14" s="8" t="n">
+        <f aca="false">R14/10</f>
+        <v>960078.6</v>
+      </c>
+      <c r="U14" s="3" t="n">
+        <f aca="false">R14/(V14/Q14)</f>
+        <v>10.4008515</v>
+      </c>
+      <c r="V14" s="1" t="n">
+        <v>1200000000</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1260,46 +1372,40 @@
         <f aca="false">A14+1</f>
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F15" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G15" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>1048576</v>
-      </c>
-      <c r="I15" s="0" t="s">
-        <v>44</v>
-      </c>
       <c r="J15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
       <c r="N15" s="0" t="n">
         <v>0</v>
       </c>
@@ -1307,11 +1413,28 @@
         <v>0</v>
       </c>
       <c r="P15" s="1" t="n">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="Q15" s="8" t="n">
-        <f aca="false">Q$4</f>
-        <v>3700</v>
+        <v>1000</v>
+      </c>
+      <c r="R15" s="8" t="n">
+        <v>13128562</v>
+      </c>
+      <c r="S15" s="9" t="n">
+        <f aca="false">V15/T15</f>
+        <v>914.037653171764</v>
+      </c>
+      <c r="T15" s="8" t="n">
+        <f aca="false">R15/10</f>
+        <v>1312856.2</v>
+      </c>
+      <c r="U15" s="3" t="n">
+        <f aca="false">R15/(V15/Q15)</f>
+        <v>10.9404683333333</v>
+      </c>
+      <c r="V15" s="1" t="n">
+        <v>1200000000</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1319,58 +1442,69 @@
         <f aca="false">A15+1</f>
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>39</v>
+      <c r="B16" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F16" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G16" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F16" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G16" s="7" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>1048576</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="J16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
       <c r="N16" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="O16" s="0" t="n">
+      <c r="O16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="P16" s="1" t="n">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="Q16" s="8" t="n">
-        <f aca="false">Q$5</f>
-        <v>2500</v>
+        <v>450</v>
+      </c>
+      <c r="R16" s="8" t="n">
+        <v>26884757</v>
+      </c>
+      <c r="S16" s="9" t="n">
+        <f aca="false">V16/T16</f>
+        <v>446.349580172884</v>
+      </c>
+      <c r="T16" s="8" t="n">
+        <f aca="false">R16/10</f>
+        <v>2688475.7</v>
+      </c>
+      <c r="U16" s="3" t="n">
+        <f aca="false">R16/(V16/Q16)</f>
+        <v>10.081783875</v>
+      </c>
+      <c r="V16" s="1" t="n">
+        <v>1200000000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1379,10 +1513,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D17" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1404,7 +1538,7 @@
         <v>1048576</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>25</v>
@@ -1412,12 +1546,8 @@
       <c r="K17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
       <c r="N17" s="0" t="n">
         <v>0</v>
       </c>
@@ -1428,7 +1558,7 @@
         <v>100</v>
       </c>
       <c r="Q17" s="8" t="n">
-        <f aca="false">Q$6</f>
+        <f aca="false">Q$13</f>
         <v>1700</v>
       </c>
     </row>
@@ -1438,10 +1568,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D18" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1474,9 +1604,7 @@
       <c r="L18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M18" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="M18" s="1"/>
       <c r="N18" s="0" t="n">
         <v>0</v>
       </c>
@@ -1484,11 +1612,11 @@
         <v>0</v>
       </c>
       <c r="P18" s="1" t="n">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="Q18" s="8" t="n">
-        <f aca="false">Q$7</f>
-        <v>1300</v>
+        <f aca="false">Q$13</f>
+        <v>1700</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1497,10 +1625,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D19" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1522,7 +1650,7 @@
         <v>1048576</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>25</v>
@@ -1543,11 +1671,11 @@
         <v>0</v>
       </c>
       <c r="P19" s="1" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="Q19" s="8" t="n">
-        <f aca="false">Q$8</f>
-        <v>1000</v>
+        <f aca="false">Q$13</f>
+        <v>1700</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1556,10 +1684,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D20" s="7" t="n">
         <f aca="false">FALSE()</f>
@@ -1581,216 +1709,1039 @@
         <v>1048576</v>
       </c>
       <c r="I20" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="P20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="0" t="n">
+        <f aca="false">Q$5</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <f aca="false">A20+1</f>
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F21" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="N21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="P21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="0" t="n">
+        <f aca="false">Q$5</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <f aca="false">A21+1</f>
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G22" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="P22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="0" t="n">
+        <f aca="false">Q$5</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <f aca="false">A22+1</f>
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="N20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="Q20" s="8" t="n">
+      <c r="D23" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F23" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q23" s="8" t="n">
         <f aca="false">Q$9</f>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="S21" s="0"/>
-      <c r="U21" s="0"/>
-      <c r="V21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
-      <c r="S22" s="0"/>
-      <c r="U22" s="0"/>
-      <c r="V22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
-      <c r="S23" s="0"/>
-      <c r="U23" s="0"/>
-      <c r="V23" s="0"/>
+        <v>210000</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
-      <c r="S24" s="0"/>
-      <c r="U24" s="0"/>
-      <c r="V24" s="0"/>
+      <c r="A24" s="0" t="n">
+        <f aca="false">A23+1</f>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F24" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G24" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q24" s="8" t="n">
+        <f aca="false">Q$10</f>
+        <v>15000</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
-      <c r="S25" s="0"/>
-      <c r="U25" s="0"/>
-      <c r="V25" s="0"/>
+      <c r="A25" s="0" t="n">
+        <f aca="false">A24+1</f>
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E25" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F25" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G25" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="Q25" s="8" t="n">
+        <f aca="false">Q$11</f>
+        <v>3700</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="S26" s="0"/>
-      <c r="U26" s="0"/>
-      <c r="V26" s="0"/>
+      <c r="A26" s="0" t="n">
+        <f aca="false">A25+1</f>
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E26" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G26" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P26" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="Q26" s="8" t="n">
+        <f aca="false">Q$12</f>
+        <v>2500</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="S27" s="0"/>
-      <c r="U27" s="0"/>
-      <c r="V27" s="0"/>
+      <c r="A27" s="0" t="n">
+        <f aca="false">A26+1</f>
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F27" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G27" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P27" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="Q27" s="8" t="n">
+        <f aca="false">Q$13</f>
+        <v>1700</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
+      <c r="A28" s="0" t="n">
+        <f aca="false">A27+1</f>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F28" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G28" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P28" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="Q28" s="8" t="n">
+        <f aca="false">Q$14</f>
+        <v>1300</v>
+      </c>
       <c r="S28" s="0"/>
       <c r="U28" s="0"/>
       <c r="V28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
+      <c r="A29" s="0" t="n">
+        <f aca="false">A28+1</f>
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F29" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G29" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I29" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P29" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="Q29" s="8" t="n">
+        <f aca="false">Q$15</f>
+        <v>1000</v>
+      </c>
+      <c r="S29" s="0"/>
+      <c r="U29" s="0"/>
+      <c r="V29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
+      <c r="A30" s="0" t="n">
+        <f aca="false">A29+1</f>
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F30" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G30" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P30" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="Q30" s="8" t="n">
+        <f aca="false">Q$16</f>
+        <v>450</v>
+      </c>
+      <c r="S30" s="0"/>
+      <c r="U30" s="0"/>
+      <c r="V30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
+      <c r="A31" s="0" t="n">
+        <f aca="false">A30+1</f>
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F31" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G31" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I31" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="P31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="0" t="n">
+        <f aca="false">Q$2</f>
+        <v>10000</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
+      <c r="A32" s="0" t="n">
+        <f aca="false">A31+1</f>
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F32" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G32" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="P32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="0" t="n">
+        <f aca="false">Q$3</f>
+        <v>9000</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
+      <c r="A33" s="0" t="n">
+        <f aca="false">A32+1</f>
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F33" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G33" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="P33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="0" t="n">
+        <f aca="false">Q$4</f>
+        <v>2250</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
+      <c r="A34" s="0" t="n">
+        <f aca="false">A33+1</f>
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E34" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F34" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G34" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="P34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="0" t="n">
+        <f aca="false">Q$5</f>
+        <v>600</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
+      <c r="A35" s="0" t="n">
+        <f aca="false">A34+1</f>
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G35" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I35" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" s="0" t="n">
+        <v>4000</v>
+      </c>
+      <c r="P35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="0" t="n">
+        <f aca="false">Q$6</f>
+        <v>150</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
-      <c r="O36" s="1"/>
-      <c r="P36" s="1"/>
+      <c r="A36" s="0" t="n">
+        <f aca="false">A35+1</f>
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F36" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G36" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" s="0" t="n">
+        <v>6000</v>
+      </c>
+      <c r="P36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="0" t="n">
+        <f aca="false">Q$7</f>
+        <v>65</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
+      <c r="A37" s="0" t="n">
+        <f aca="false">A36+1</f>
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F37" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G37" s="7" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" s="0" t="n">
+        <v>8000</v>
+      </c>
+      <c r="P37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="0" t="n">
+        <f aca="false">Q$8</f>
+        <v>40</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0"/>
@@ -1804,8 +2755,6 @@
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
@@ -2274,18 +3223,9 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="7"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="O70" s="1"/>
-      <c r="P70" s="1"/>
+      <c r="S70" s="0"/>
+      <c r="U70" s="0"/>
+      <c r="V70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0"/>

</xml_diff>